<commit_message>
2023 longevity data added as csv file
</commit_message>
<xml_diff>
--- a/results/models significances.xlsx
+++ b/results/models significances.xlsx
@@ -1,36 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\laptop\OneDrive - Universidad de Oviedo\IMIB\Softwares\GitHub\ageing\results\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://unioviedo-my.sharepoint.com/personal/espinosaclara_uniovi_es/Documents/IMIB/Softwares/GitHub/ageing/results/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="2" documentId="11_6CB6C5C6904DE05BCC18679270FD9BBCF7AC8D37" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{CF6152A9-1CAA-4B8D-B296-C1B710A881E9}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="-19665" yWindow="855" windowWidth="14850" windowHeight="11250"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="multinomial models" sheetId="1" r:id="rId1"/>
     <sheet name="gaussian models" sheetId="3" r:id="rId2"/>
     <sheet name="overall percentages" sheetId="2" r:id="rId3"/>
-    <sheet name="genstat parameters" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -237,7 +227,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -383,7 +373,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="11" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -397,19 +386,20 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="2" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -723,10 +713,10 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:O45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="M12" sqref="M12"/>
     </sheetView>
   </sheetViews>
@@ -751,13 +741,13 @@
       </c>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A2" s="6" t="s">
+      <c r="A2" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="D2" s="6" t="s">
+      <c r="D2" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="H2" s="6" t="s">
+      <c r="H2" s="5" t="s">
         <v>42</v>
       </c>
     </row>
@@ -837,7 +827,7 @@
       <c r="H6" t="s">
         <v>4</v>
       </c>
-      <c r="I6" s="3">
+      <c r="I6">
         <v>0.14799999999999999</v>
       </c>
     </row>
@@ -897,82 +887,82 @@
       <c r="H9" t="s">
         <v>8</v>
       </c>
-      <c r="I9" s="3">
+      <c r="I9">
         <v>0.63700000000000001</v>
       </c>
-      <c r="K9" s="18" t="s">
+      <c r="K9" s="17" t="s">
         <v>55</v>
       </c>
-      <c r="L9" s="18" t="s">
+      <c r="L9" s="17" t="s">
         <v>13</v>
       </c>
-      <c r="M9" s="18" t="s">
+      <c r="M9" s="17" t="s">
         <v>49</v>
       </c>
-      <c r="N9" s="18" t="s">
+      <c r="N9" s="17" t="s">
         <v>56</v>
       </c>
-      <c r="O9" s="18" t="s">
+      <c r="O9" s="17" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="K10" s="20" t="s">
+      <c r="K10" s="19" t="s">
         <v>50</v>
       </c>
-      <c r="L10" s="18" t="s">
+      <c r="L10" s="17" t="s">
         <v>63</v>
       </c>
-      <c r="M10" s="18" t="s">
+      <c r="M10" s="17" t="s">
         <v>60</v>
       </c>
-      <c r="N10" s="19" t="s">
+      <c r="N10" s="18" t="s">
         <v>54</v>
       </c>
-      <c r="O10" s="18" t="s">
+      <c r="O10" s="17" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="K11" s="20" t="s">
+      <c r="K11" s="19" t="s">
         <v>51</v>
       </c>
-      <c r="L11" s="18" t="s">
+      <c r="L11" s="17" t="s">
         <v>63</v>
       </c>
-      <c r="M11" s="19" t="s">
+      <c r="M11" s="18" t="s">
         <v>54</v>
       </c>
-      <c r="N11" s="18" t="s">
+      <c r="N11" s="17" t="s">
         <v>59</v>
       </c>
-      <c r="O11" s="18" t="s">
+      <c r="O11" s="17" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A12" s="6" t="s">
+      <c r="A12" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="D12" s="6" t="s">
+      <c r="D12" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="H12" s="6" t="s">
+      <c r="H12" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="K12" s="20" t="s">
+      <c r="K12" s="19" t="s">
         <v>57</v>
       </c>
-      <c r="L12" s="18" t="s">
+      <c r="L12" s="17" t="s">
         <v>63</v>
       </c>
-      <c r="M12" s="18" t="s">
+      <c r="M12" s="17" t="s">
         <v>62</v>
       </c>
-      <c r="N12" s="18" t="s">
+      <c r="N12" s="17" t="s">
         <v>61</v>
       </c>
-      <c r="O12" s="18" t="s">
+      <c r="O12" s="17" t="s">
         <v>64</v>
       </c>
     </row>
@@ -1078,23 +1068,23 @@
     </row>
     <row r="19" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A20" s="7" t="s">
+      <c r="A20" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="B20" s="8"/>
-      <c r="D20" s="6" t="s">
+      <c r="B20" s="7"/>
+      <c r="D20" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="H20" s="7" t="s">
+      <c r="H20" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="I20" s="8"/>
+      <c r="I20" s="7"/>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A21" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="B21" s="10" t="s">
+      <c r="A21" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="B21" s="9" t="s">
         <v>0</v>
       </c>
       <c r="D21" t="s">
@@ -1103,18 +1093,18 @@
       <c r="E21" t="s">
         <v>0</v>
       </c>
-      <c r="H21" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="I21" s="10" t="s">
+      <c r="H21" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="I21" s="9" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A22" s="9" t="s">
+      <c r="A22" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="B22" s="10">
+      <c r="B22" s="9">
         <v>0.43911</v>
       </c>
       <c r="D22" t="s">
@@ -1123,18 +1113,18 @@
       <c r="E22" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="H22" s="9" t="s">
+      <c r="H22" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="I22" s="10">
+      <c r="I22" s="9">
         <v>0.45800000000000002</v>
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A23" s="9" t="s">
+      <c r="A23" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="B23" s="11" t="s">
+      <c r="B23" s="10" t="s">
         <v>11</v>
       </c>
       <c r="D23" t="s">
@@ -1143,18 +1133,18 @@
       <c r="E23" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="H23" s="9" t="s">
+      <c r="H23" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="I23" s="11" t="s">
+      <c r="I23" s="10" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A24" s="9" t="s">
+      <c r="A24" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="B24" s="12">
+      <c r="B24" s="11">
         <v>5.6669999999999998E-2</v>
       </c>
       <c r="D24" t="s">
@@ -1163,38 +1153,38 @@
       <c r="E24" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="H24" s="9" t="s">
+      <c r="H24" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="I24" s="12">
+      <c r="I24" s="11">
         <v>6.9000000000000006E-2</v>
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A25" s="9" t="s">
+      <c r="A25" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="B25" s="10">
+      <c r="B25" s="9">
         <v>0.52156000000000002</v>
       </c>
       <c r="D25" t="s">
         <v>5</v>
       </c>
-      <c r="E25" s="4">
+      <c r="E25" s="3">
         <v>7.54E-8</v>
       </c>
-      <c r="H25" s="9" t="s">
+      <c r="H25" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="I25" s="10">
+      <c r="I25" s="9">
         <v>0.72699999999999998</v>
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A26" s="9" t="s">
+      <c r="A26" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="B26" s="10">
+      <c r="B26" s="9">
         <v>0.79378000000000004</v>
       </c>
       <c r="D26" t="s">
@@ -1203,38 +1193,38 @@
       <c r="E26">
         <v>0.38300000000000001</v>
       </c>
-      <c r="H26" s="9" t="s">
+      <c r="H26" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="I26" s="10">
+      <c r="I26" s="9">
         <v>0.25889000000000001</v>
       </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A27" s="9" t="s">
+      <c r="A27" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="B27" s="11">
+      <c r="B27" s="10">
         <v>5.5599999999999998E-3</v>
       </c>
       <c r="D27" t="s">
         <v>14</v>
       </c>
-      <c r="E27" s="3">
+      <c r="E27">
         <v>0.96299999999999997</v>
       </c>
-      <c r="H27" s="9" t="s">
+      <c r="H27" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="I27" s="11">
+      <c r="I27" s="10">
         <v>3.3E-3</v>
       </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A28" s="9" t="s">
+      <c r="A28" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="B28" s="10">
+      <c r="B28" s="9">
         <v>0.13711000000000001</v>
       </c>
       <c r="D28" t="s">
@@ -1243,41 +1233,41 @@
       <c r="E28">
         <v>0.624</v>
       </c>
-      <c r="H28" s="9" t="s">
+      <c r="H28" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="I28" s="10">
+      <c r="I28" s="9">
         <v>0.52600000000000002</v>
       </c>
     </row>
     <row r="29" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="13" t="s">
+      <c r="A29" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="B29" s="14">
+      <c r="B29" s="13">
         <v>7.0669999999999997E-2</v>
       </c>
       <c r="D29" t="s">
         <v>16</v>
       </c>
-      <c r="E29" s="4">
+      <c r="E29" s="3">
         <v>5.9599999999999999E-5</v>
       </c>
-      <c r="H29" s="13" t="s">
+      <c r="H29" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="I29" s="14">
+      <c r="I29" s="13">
         <v>0.61899999999999999</v>
       </c>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A32" s="6" t="s">
+      <c r="A32" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="D32" s="6" t="s">
+      <c r="D32" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="H32" s="6" t="s">
+      <c r="H32" s="5" t="s">
         <v>45</v>
       </c>
     </row>
@@ -1305,19 +1295,19 @@
       <c r="A34" t="s">
         <v>1</v>
       </c>
-      <c r="B34" s="3">
+      <c r="B34">
         <v>0.51819999999999999</v>
       </c>
       <c r="D34" t="s">
         <v>1</v>
       </c>
-      <c r="E34" s="3">
+      <c r="E34">
         <v>0.30199999999999999</v>
       </c>
       <c r="H34" t="s">
         <v>1</v>
       </c>
-      <c r="I34" s="3">
+      <c r="I34">
         <v>0.52490000000000003</v>
       </c>
     </row>
@@ -1345,19 +1335,19 @@
       <c r="A36" t="s">
         <v>27</v>
       </c>
-      <c r="B36" s="3">
+      <c r="B36">
         <v>0.77090000000000003</v>
       </c>
       <c r="D36" t="s">
         <v>27</v>
       </c>
-      <c r="E36" s="3">
+      <c r="E36">
         <v>0.98899999999999999</v>
       </c>
       <c r="H36" t="s">
         <v>27</v>
       </c>
-      <c r="I36" s="3">
+      <c r="I36">
         <v>0.72640000000000005</v>
       </c>
     </row>
@@ -1365,19 +1355,19 @@
       <c r="A37" t="s">
         <v>28</v>
       </c>
-      <c r="B37" s="4">
+      <c r="B37" s="3">
         <v>3.3599999999999998E-2</v>
       </c>
       <c r="D37" t="s">
         <v>28</v>
       </c>
-      <c r="E37" s="4">
+      <c r="E37" s="3">
         <v>0.378</v>
       </c>
       <c r="H37" t="s">
         <v>28</v>
       </c>
-      <c r="I37" s="16">
+      <c r="I37" s="15">
         <v>4.7300000000000002E-2</v>
       </c>
     </row>
@@ -1385,19 +1375,19 @@
       <c r="A38" t="s">
         <v>29</v>
       </c>
-      <c r="B38" s="3">
+      <c r="B38">
         <v>0.27800000000000002</v>
       </c>
       <c r="D38" t="s">
         <v>29</v>
       </c>
-      <c r="E38" s="3">
+      <c r="E38">
         <v>0.38900000000000001</v>
       </c>
       <c r="H38" t="s">
         <v>30</v>
       </c>
-      <c r="I38" s="3">
+      <c r="I38">
         <v>0.32290000000000002</v>
       </c>
     </row>
@@ -1405,19 +1395,19 @@
       <c r="A39" t="s">
         <v>30</v>
       </c>
-      <c r="B39" s="3">
+      <c r="B39">
         <v>0.4551</v>
       </c>
       <c r="D39" t="s">
         <v>30</v>
       </c>
-      <c r="E39" s="3">
+      <c r="E39">
         <v>0.71299999999999997</v>
       </c>
       <c r="H39" t="s">
         <v>32</v>
       </c>
-      <c r="I39" s="3">
+      <c r="I39">
         <v>0.52529999999999999</v>
       </c>
     </row>
@@ -1425,13 +1415,13 @@
       <c r="A40" t="s">
         <v>31</v>
       </c>
-      <c r="B40" s="3">
+      <c r="B40">
         <v>0.17130000000000001</v>
       </c>
       <c r="D40" t="s">
         <v>31</v>
       </c>
-      <c r="E40" s="3">
+      <c r="E40">
         <v>0.26200000000000001</v>
       </c>
       <c r="H40" t="s">
@@ -1445,19 +1435,19 @@
       <c r="A41" t="s">
         <v>32</v>
       </c>
-      <c r="B41" s="4">
+      <c r="B41" s="3">
         <v>0.51400000000000001</v>
       </c>
       <c r="D41" t="s">
         <v>32</v>
       </c>
-      <c r="E41" s="4">
+      <c r="E41" s="3">
         <v>0.52200000000000002</v>
       </c>
       <c r="H41" t="s">
         <v>34</v>
       </c>
-      <c r="I41" s="17">
+      <c r="I41" s="16">
         <v>0.8236</v>
       </c>
     </row>
@@ -1474,52 +1464,48 @@
       <c r="E42" s="1">
         <v>2.1999999999999999E-2</v>
       </c>
-      <c r="I42" s="3"/>
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>33</v>
       </c>
-      <c r="B43" s="3">
+      <c r="B43">
         <v>0.72640000000000005</v>
       </c>
       <c r="D43" t="s">
         <v>33</v>
       </c>
-      <c r="E43" s="3">
+      <c r="E43">
         <v>0.72699999999999998</v>
       </c>
-      <c r="I43" s="3"/>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>34</v>
       </c>
-      <c r="B44" s="3">
+      <c r="B44">
         <v>0.3296</v>
       </c>
       <c r="D44" t="s">
         <v>34</v>
       </c>
-      <c r="E44" s="3">
+      <c r="E44">
         <v>0.32100000000000001</v>
       </c>
-      <c r="I44" s="3"/>
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>35</v>
       </c>
-      <c r="B45" s="3">
+      <c r="B45">
         <v>0.72960000000000003</v>
       </c>
       <c r="D45" t="s">
         <v>35</v>
       </c>
-      <c r="E45" s="3">
+      <c r="E45">
         <v>0.73499999999999999</v>
       </c>
-      <c r="I45" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1527,10 +1513,10 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:Q41"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
@@ -1552,40 +1538,40 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A1" s="15" t="s">
+      <c r="A1" s="14" t="s">
         <v>38</v>
       </c>
-      <c r="B1" s="21" t="s">
+      <c r="B1" s="20" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="21"/>
-      <c r="D1" s="21"/>
+      <c r="C1" s="20"/>
+      <c r="D1" s="20"/>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="B2" s="6"/>
+      <c r="B2" s="5"/>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>39</v>
       </c>
-      <c r="B3" s="5" t="s">
+      <c r="B3" s="4" t="s">
         <v>37</v>
       </c>
       <c r="D3" t="s">
         <v>39</v>
       </c>
-      <c r="E3" s="5" t="s">
+      <c r="E3" s="4" t="s">
         <v>41</v>
       </c>
       <c r="G3" t="s">
         <v>39</v>
       </c>
-      <c r="H3" s="5" t="s">
+      <c r="H3" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="K3" s="5"/>
-      <c r="N3" s="5"/>
-      <c r="Q3" s="5"/>
+      <c r="K3" s="4"/>
+      <c r="N3" s="4"/>
+      <c r="Q3" s="4"/>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
@@ -1603,12 +1589,9 @@
       <c r="G4" t="s">
         <v>10</v>
       </c>
-      <c r="H4" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="K4" s="3"/>
-      <c r="N4" s="3"/>
-      <c r="Q4" s="3"/>
+      <c r="H4" t="s">
+        <v>0</v>
+      </c>
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
@@ -1620,18 +1603,15 @@
       <c r="D5" t="s">
         <v>1</v>
       </c>
-      <c r="E5" s="3">
+      <c r="E5">
         <v>0.80400000000000005</v>
       </c>
       <c r="G5" t="s">
         <v>1</v>
       </c>
-      <c r="H5" s="3">
+      <c r="H5">
         <v>0.42699999999999999</v>
       </c>
-      <c r="K5" s="3"/>
-      <c r="N5" s="3"/>
-      <c r="Q5" s="3"/>
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
@@ -1643,18 +1623,15 @@
       <c r="D6" t="s">
         <v>3</v>
       </c>
-      <c r="E6" s="3">
+      <c r="E6">
         <v>0.89400000000000002</v>
       </c>
       <c r="G6" t="s">
         <v>3</v>
       </c>
-      <c r="H6" s="3">
+      <c r="H6">
         <v>0.56499999999999995</v>
       </c>
-      <c r="K6" s="3"/>
-      <c r="N6" s="3"/>
-      <c r="Q6" s="3"/>
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
@@ -1666,18 +1643,15 @@
       <c r="D7" t="s">
         <v>4</v>
       </c>
-      <c r="E7" s="3">
+      <c r="E7">
         <v>0.90200000000000002</v>
       </c>
       <c r="G7" t="s">
         <v>4</v>
       </c>
-      <c r="H7" s="3">
+      <c r="H7">
         <v>0.89200000000000002</v>
       </c>
-      <c r="K7" s="3"/>
-      <c r="N7" s="3"/>
-      <c r="Q7" s="3"/>
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
@@ -1689,18 +1663,15 @@
       <c r="D8" t="s">
         <v>5</v>
       </c>
-      <c r="E8" s="3">
+      <c r="E8">
         <v>0.95499999999999996</v>
       </c>
       <c r="G8" t="s">
         <v>5</v>
       </c>
-      <c r="H8" s="3">
+      <c r="H8">
         <v>0.65900000000000003</v>
       </c>
-      <c r="K8" s="3"/>
-      <c r="N8" s="3"/>
-      <c r="Q8" s="3"/>
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
@@ -1712,41 +1683,35 @@
       <c r="D9" t="s">
         <v>6</v>
       </c>
-      <c r="E9" s="3">
+      <c r="E9">
         <v>0.78300000000000003</v>
       </c>
       <c r="G9" t="s">
         <v>6</v>
       </c>
-      <c r="H9" s="3">
+      <c r="H9">
         <v>0.34399999999999997</v>
       </c>
-      <c r="K9" s="3"/>
-      <c r="N9" s="3"/>
-      <c r="Q9" s="3"/>
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>7</v>
       </c>
-      <c r="B10" s="1">
+      <c r="B10" s="21">
         <v>7.3300000000000004E-2</v>
       </c>
       <c r="D10" t="s">
         <v>7</v>
       </c>
-      <c r="E10" s="3">
+      <c r="E10">
         <v>0.92800000000000005</v>
       </c>
       <c r="G10" t="s">
         <v>7</v>
       </c>
-      <c r="H10" s="3">
+      <c r="H10">
         <v>0.83599999999999997</v>
       </c>
-      <c r="K10" s="3"/>
-      <c r="N10" s="3"/>
-      <c r="Q10" s="3"/>
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
@@ -1758,18 +1723,15 @@
       <c r="D11" t="s">
         <v>8</v>
       </c>
-      <c r="E11" s="3">
+      <c r="E11">
         <v>0.97499999999999998</v>
       </c>
       <c r="G11" t="s">
         <v>8</v>
       </c>
-      <c r="H11" s="3">
+      <c r="H11">
         <v>0.56000000000000005</v>
       </c>
-      <c r="K11" s="3"/>
-      <c r="N11" s="3"/>
-      <c r="Q11" s="3"/>
     </row>
     <row r="12" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
@@ -1781,49 +1743,46 @@
       <c r="D12" t="s">
         <v>9</v>
       </c>
-      <c r="E12" s="3">
+      <c r="E12">
         <v>0.97399999999999998</v>
       </c>
       <c r="G12" t="s">
         <v>9</v>
       </c>
-      <c r="H12" s="3">
+      <c r="H12">
         <v>0.88800000000000001</v>
       </c>
-      <c r="K12" s="3"/>
-      <c r="N12" s="3"/>
-      <c r="Q12" s="3"/>
     </row>
     <row r="15" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A15" s="15" t="s">
+      <c r="A15" s="14" t="s">
         <v>38</v>
       </c>
-      <c r="B15" s="21" t="s">
+      <c r="B15" s="20" t="s">
         <v>42</v>
       </c>
-      <c r="C15" s="21"/>
-      <c r="D15" s="21"/>
+      <c r="C15" s="20"/>
+      <c r="D15" s="20"/>
     </row>
     <row r="16" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="B16" s="6"/>
+      <c r="B16" s="5"/>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>39</v>
       </c>
-      <c r="B17" s="5" t="s">
+      <c r="B17" s="4" t="s">
         <v>37</v>
       </c>
       <c r="D17" t="s">
         <v>39</v>
       </c>
-      <c r="E17" s="5" t="s">
+      <c r="E17" s="4" t="s">
         <v>41</v>
       </c>
       <c r="G17" t="s">
         <v>39</v>
       </c>
-      <c r="H17" s="5" t="s">
+      <c r="H17" s="4" t="s">
         <v>40</v>
       </c>
     </row>
@@ -1843,7 +1802,7 @@
       <c r="G18" t="s">
         <v>10</v>
       </c>
-      <c r="H18" s="3" t="s">
+      <c r="H18" t="s">
         <v>0</v>
       </c>
     </row>
@@ -1857,13 +1816,13 @@
       <c r="D19" t="s">
         <v>1</v>
       </c>
-      <c r="E19" s="3">
+      <c r="E19">
         <v>0.77769999999999995</v>
       </c>
       <c r="G19" t="s">
         <v>1</v>
       </c>
-      <c r="H19" s="3">
+      <c r="H19">
         <v>0.42599999999999999</v>
       </c>
     </row>
@@ -1877,13 +1836,13 @@
       <c r="D20" t="s">
         <v>3</v>
       </c>
-      <c r="E20" s="3">
+      <c r="E20">
         <v>0.90800000000000003</v>
       </c>
       <c r="G20" t="s">
         <v>3</v>
       </c>
-      <c r="H20" s="3">
+      <c r="H20">
         <v>0.58199999999999996</v>
       </c>
     </row>
@@ -1897,13 +1856,13 @@
       <c r="D21" t="s">
         <v>4</v>
       </c>
-      <c r="E21" s="3">
+      <c r="E21">
         <v>0.93600000000000005</v>
       </c>
       <c r="G21" t="s">
         <v>4</v>
       </c>
-      <c r="H21" s="3">
+      <c r="H21">
         <v>0.93899999999999995</v>
       </c>
     </row>
@@ -1917,13 +1876,13 @@
       <c r="D22" t="s">
         <v>5</v>
       </c>
-      <c r="E22" s="3">
+      <c r="E22">
         <v>0.997</v>
       </c>
       <c r="G22" t="s">
         <v>5</v>
       </c>
-      <c r="H22" s="3">
+      <c r="H22">
         <v>0.85</v>
       </c>
     </row>
@@ -1937,13 +1896,13 @@
       <c r="D23" t="s">
         <v>7</v>
       </c>
-      <c r="E23" s="3">
+      <c r="E23">
         <v>0.94399999999999995</v>
       </c>
       <c r="G23" t="s">
         <v>7</v>
       </c>
-      <c r="H23" s="3">
+      <c r="H23">
         <v>0.78300000000000003</v>
       </c>
     </row>
@@ -1957,46 +1916,46 @@
       <c r="D24" t="s">
         <v>8</v>
       </c>
-      <c r="E24" s="3">
+      <c r="E24">
         <v>0.99299999999999999</v>
       </c>
       <c r="G24" t="s">
         <v>8</v>
       </c>
-      <c r="H24" s="3">
+      <c r="H24">
         <v>0.53900000000000003</v>
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A27" s="15" t="s">
+      <c r="A27" s="14" t="s">
         <v>38</v>
       </c>
-      <c r="B27" s="21" t="s">
+      <c r="B27" s="20" t="s">
         <v>44</v>
       </c>
-      <c r="C27" s="21"/>
-      <c r="D27" s="21"/>
+      <c r="C27" s="20"/>
+      <c r="D27" s="20"/>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B28" s="6"/>
+      <c r="B28" s="5"/>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>39</v>
       </c>
-      <c r="B29" s="5" t="s">
+      <c r="B29" s="4" t="s">
         <v>37</v>
       </c>
       <c r="D29" t="s">
         <v>39</v>
       </c>
-      <c r="E29" s="5" t="s">
+      <c r="E29" s="4" t="s">
         <v>41</v>
       </c>
       <c r="G29" t="s">
         <v>39</v>
       </c>
-      <c r="H29" s="5" t="s">
+      <c r="H29" s="4" t="s">
         <v>40</v>
       </c>
     </row>
@@ -2016,7 +1975,7 @@
       <c r="G30" t="s">
         <v>10</v>
       </c>
-      <c r="H30" s="3" t="s">
+      <c r="H30" t="s">
         <v>0</v>
       </c>
     </row>
@@ -2030,13 +1989,13 @@
       <c r="D31" t="s">
         <v>1</v>
       </c>
-      <c r="E31" s="3">
+      <c r="E31">
         <v>0.76300000000000001</v>
       </c>
       <c r="G31" t="s">
         <v>1</v>
       </c>
-      <c r="H31" s="3">
+      <c r="H31">
         <v>0.44400000000000001</v>
       </c>
     </row>
@@ -2050,13 +2009,13 @@
       <c r="D32" t="s">
         <v>3</v>
       </c>
-      <c r="E32" s="3">
+      <c r="E32">
         <v>0.86499999999999999</v>
       </c>
       <c r="G32" t="s">
         <v>3</v>
       </c>
-      <c r="H32" s="3">
+      <c r="H32">
         <v>0.20799999999999999</v>
       </c>
     </row>
@@ -2070,13 +2029,13 @@
       <c r="D33" t="s">
         <v>6</v>
       </c>
-      <c r="E33" s="3">
+      <c r="E33">
         <v>0.80600000000000005</v>
       </c>
       <c r="G33" t="s">
         <v>6</v>
       </c>
-      <c r="H33" s="3">
+      <c r="H33">
         <v>0.30399999999999999</v>
       </c>
     </row>
@@ -2090,46 +2049,46 @@
       <c r="D34" t="s">
         <v>9</v>
       </c>
-      <c r="E34" s="3">
+      <c r="E34">
         <v>0.94499999999999995</v>
       </c>
       <c r="G34" t="s">
         <v>9</v>
       </c>
-      <c r="H34" s="3">
+      <c r="H34">
         <v>0.83599999999999997</v>
       </c>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A36" s="15" t="s">
+      <c r="A36" s="14" t="s">
         <v>38</v>
       </c>
-      <c r="B36" s="21" t="s">
+      <c r="B36" s="20" t="s">
         <v>3</v>
       </c>
-      <c r="C36" s="21"/>
-      <c r="D36" s="21"/>
+      <c r="C36" s="20"/>
+      <c r="D36" s="20"/>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B37" s="6"/>
+      <c r="B37" s="5"/>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>39</v>
       </c>
-      <c r="B38" s="5" t="s">
+      <c r="B38" s="4" t="s">
         <v>37</v>
       </c>
       <c r="D38" t="s">
         <v>39</v>
       </c>
-      <c r="E38" s="5" t="s">
+      <c r="E38" s="4" t="s">
         <v>41</v>
       </c>
       <c r="G38" t="s">
         <v>39</v>
       </c>
-      <c r="H38" s="5" t="s">
+      <c r="H38" s="4" t="s">
         <v>40</v>
       </c>
     </row>
@@ -2149,7 +2108,7 @@
       <c r="G39" t="s">
         <v>10</v>
       </c>
-      <c r="H39" s="3" t="s">
+      <c r="H39" t="s">
         <v>0</v>
       </c>
     </row>
@@ -2163,13 +2122,13 @@
       <c r="D40" t="s">
         <v>1</v>
       </c>
-      <c r="E40" s="3">
+      <c r="E40">
         <v>0.72699999999999998</v>
       </c>
       <c r="G40" t="s">
         <v>1</v>
       </c>
-      <c r="H40" s="3">
+      <c r="H40">
         <v>0.42699999999999999</v>
       </c>
     </row>
@@ -2183,13 +2142,13 @@
       <c r="D41" t="s">
         <v>3</v>
       </c>
-      <c r="E41" s="3">
+      <c r="E41">
         <v>0.875</v>
       </c>
       <c r="G41" t="s">
         <v>3</v>
       </c>
-      <c r="H41" s="3">
+      <c r="H41">
         <v>0.16300000000000001</v>
       </c>
     </row>
@@ -2205,7 +2164,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:G16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2493,18 +2452,4 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E20" sqref="E20"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>